<commit_message>
08:45 - 03.02.2025 - 3rd and 4th week Excel's retouch
</commit_message>
<xml_diff>
--- a/NachDurchlaufplan/excelFiles/2-P&DS.xlsx
+++ b/NachDurchlaufplan/excelFiles/2-P&DS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/pit5lo_bosch_com/Documents/Ausbildung - Fachinformatik/NachDurchlaufplan/excelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="13_ncr:1_{34DBF14C-E358-4AB5-A6F9-5FA28043C4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A99384B6-C1A1-455B-A993-6E4407981067}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="13_ncr:1_{34DBF14C-E358-4AB5-A6F9-5FA28043C4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB570772-F56C-4885-83E0-E399D91098DA}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9650" windowHeight="10170" firstSheet="2" activeTab="3" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -1110,7 +1110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1268,6 +1268,12 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1277,9 +1283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1310,9 +1313,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,15 +1325,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1361,15 +1361,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1405,6 +1405,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1763,22 +1766,22 @@
       <selection activeCell="B29" sqref="B29:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39"/>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
@@ -1800,7 +1803,7 @@
       <c r="C3" s="14"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
@@ -1808,7 +1811,7 @@
       <c r="C4" s="15"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
@@ -1818,7 +1821,7 @@
       <c r="C5" s="43"/>
       <c r="D5" s="44"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
@@ -1826,7 +1829,7 @@
       <c r="C6" s="46"/>
       <c r="D6" s="47"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>0.375</v>
       </c>
@@ -1834,7 +1837,7 @@
       <c r="C7" s="15"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>0.38541666666666702</v>
       </c>
@@ -1842,7 +1845,7 @@
       <c r="C8" s="15"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>0.39583333333333298</v>
       </c>
@@ -1850,7 +1853,7 @@
       <c r="C9" s="15"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>0.40625</v>
       </c>
@@ -1858,7 +1861,7 @@
       <c r="C10" s="15"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>0.41666666666666702</v>
       </c>
@@ -1866,7 +1869,7 @@
       <c r="C11" s="15"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>0.42708333333333298</v>
       </c>
@@ -1874,7 +1877,7 @@
       <c r="C12" s="15"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>0.4375</v>
       </c>
@@ -1882,7 +1885,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>0.44791666666666702</v>
       </c>
@@ -1890,7 +1893,7 @@
       <c r="C14" s="15"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>0.45833333333333298</v>
       </c>
@@ -1898,7 +1901,7 @@
       <c r="C15" s="15"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>0.46875</v>
       </c>
@@ -1906,7 +1909,7 @@
       <c r="C16" s="15"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>0.47916666666666702</v>
       </c>
@@ -1914,7 +1917,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>0.48958333333333298</v>
       </c>
@@ -1922,7 +1925,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <v>0.5</v>
       </c>
@@ -1932,25 +1935,25 @@
       <c r="C19" s="48"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="52"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>0.54166666666666696</v>
       </c>
@@ -1958,7 +1961,7 @@
       <c r="C23" s="15"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>0.55208333333333304</v>
       </c>
@@ -1966,7 +1969,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>0.5625</v>
       </c>
@@ -1974,7 +1977,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>0.57291666666666696</v>
       </c>
@@ -1982,7 +1985,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>0.58333333333333304</v>
       </c>
@@ -1990,7 +1993,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>0.59375</v>
       </c>
@@ -1998,7 +2001,7 @@
       <c r="C28" s="17"/>
       <c r="D28" s="21"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>0.60416666666666696</v>
       </c>
@@ -2008,7 +2011,7 @@
       <c r="C29" s="43"/>
       <c r="D29" s="44"/>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>0.61458333333333304</v>
       </c>
@@ -2036,16 +2039,16 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>17</v>
       </c>
@@ -2053,7 +2056,7 @@
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2067,27 +2070,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
@@ -2097,7 +2100,7 @@
       <c r="C5" s="43"/>
       <c r="D5" s="44"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
@@ -2105,37 +2108,37 @@
       <c r="C6" s="69"/>
       <c r="D6" s="70"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>0.375</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="61" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="20"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="61"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="57"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="30" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
@@ -2145,11 +2148,11 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="53" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="29" t="s">
@@ -2157,77 +2160,77 @@
       </c>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B12" s="57"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="30" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="57"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="67"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="31" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="59" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="59"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="21"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="61" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="24"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="62"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="25"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <v>0.5</v>
       </c>
@@ -2237,98 +2240,99 @@
       <c r="C19" s="48"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="52"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="61" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="61"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="61"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="61"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="61" t="s">
+      <c r="B27" s="65"/>
+      <c r="C27" s="62" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="61"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="62"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="62"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="63"/>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B11:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="A1:D1"/>
@@ -2345,7 +2349,6 @@
     <mergeCell ref="B5:D6"/>
     <mergeCell ref="B19:D22"/>
     <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2355,20 +2358,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C1958D-7396-4A88-8B63-5928A8A1F579}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>36</v>
       </c>
@@ -2376,7 +2379,7 @@
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2390,149 +2393,149 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="61" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="61"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="61"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>0.375</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="61"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="64"/>
-      <c r="C8" s="61"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="61"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="62"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="63"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="61" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
       <c r="B12" s="73"/>
-      <c r="C12" s="72"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="21"/>
     </row>
-    <row r="13" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="61" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="20"/>
     </row>
-    <row r="14" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="61"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="61"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="61" t="s">
+      <c r="B16" s="65"/>
+      <c r="C16" s="62" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="61"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="62"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <v>0.5</v>
       </c>
@@ -2542,29 +2545,29 @@
       <c r="C19" s="48"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="52"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="64" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="29" t="s">
@@ -2572,74 +2575,81 @@
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="64"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="61" t="s">
+      <c r="B25" s="65"/>
+      <c r="C25" s="62" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>0.57291666666666696</v>
       </c>
       <c r="B26" s="73"/>
-      <c r="C26" s="72"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="21"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="61" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="20"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="61"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="62"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="62"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="63"/>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="66"/>
-      <c r="D30" s="74"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:D22"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="B3:B10"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="B13:B18"/>
@@ -2648,13 +2658,6 @@
     <mergeCell ref="C27:C29"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:D22"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="B3:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2664,20 +2667,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838E9BEF-82DD-4851-A0DE-5B88C1E3608B}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>37</v>
       </c>
@@ -2685,7 +2688,7 @@
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2699,11 +2702,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="53" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -2711,47 +2714,47 @@
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="57"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="27" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="57"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>0.375</v>
       </c>
-      <c r="B7" s="57"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="28" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="21"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
@@ -2763,7 +2766,7 @@
       </c>
       <c r="D8" s="36"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
@@ -2771,7 +2774,7 @@
       <c r="C9" s="79"/>
       <c r="D9" s="37"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
@@ -2779,7 +2782,7 @@
       <c r="C10" s="79"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
@@ -2787,7 +2790,7 @@
       <c r="C11" s="79"/>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
@@ -2795,11 +2798,11 @@
       <c r="C12" s="80"/>
       <c r="D12" s="38"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="64" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="81" t="s">
@@ -2807,47 +2810,47 @@
       </c>
       <c r="D13" s="20"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="64"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="82"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="64"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="82"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="64"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="82"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="82"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="65"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="83"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <v>0.5</v>
       </c>
@@ -2857,109 +2860,109 @@
       <c r="C19" s="48"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="52"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="61" t="s">
         <v>57</v>
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="59"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="59"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="16"/>
-    </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="65"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="66"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="16"/>
-    </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="10">
+      <c r="B28" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="66"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="99"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="35">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="B30" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="69"/>
-      <c r="D29" s="70"/>
-    </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="11">
-        <v>0.61458333333333304</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="B19:D22"/>
-    <mergeCell ref="B29:D30"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="C8:C12"/>
     <mergeCell ref="B13:B18"/>
@@ -2973,20 +2976,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C18F7BC-573D-4430-99F0-5E921D81B802}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:D30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>38</v>
       </c>
@@ -2994,7 +2997,7 @@
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3008,151 +3011,151 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="59"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>0.375</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="59"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="21"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="84" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="20"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>0.40625</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="84"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="85"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="85" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="84"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="85"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="59" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="59"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="59"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="66"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <v>0.5</v>
       </c>
@@ -3162,98 +3165,104 @@
       <c r="C19" s="48"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="52"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="61" t="s">
         <v>61</v>
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="61"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="61"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="B26" s="65"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="61"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="62" t="s">
+        <v>62</v>
+      </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
       <c r="B28" s="65"/>
       <c r="C28" s="62"/>
-      <c r="D28" s="16"/>
-    </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="10">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="66"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="99"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="35">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="B30" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="69"/>
-      <c r="D29" s="70"/>
-    </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="11">
-        <v>0.61458333333333304</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="B19:D22"/>
@@ -3263,12 +3272,6 @@
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B29:D30"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3282,16 +3285,16 @@
       <selection activeCell="B23" sqref="B23:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>39</v>
       </c>
@@ -3299,7 +3302,7 @@
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3313,27 +3316,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="74" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>0.35416666666666702</v>
       </c>
@@ -3341,35 +3344,35 @@
       <c r="C5" s="87"/>
       <c r="D5" s="30"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="74" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="30"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>0.375</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="30"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
@@ -3377,7 +3380,7 @@
       <c r="C9" s="87"/>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
@@ -3387,7 +3390,7 @@
       <c r="C10" s="97"/>
       <c r="D10" s="98"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
@@ -3397,7 +3400,7 @@
       <c r="C11" s="89"/>
       <c r="D11" s="90"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
@@ -3405,7 +3408,7 @@
       <c r="C12" s="69"/>
       <c r="D12" s="92"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
@@ -3413,7 +3416,7 @@
       <c r="C13" s="69"/>
       <c r="D13" s="92"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
@@ -3421,7 +3424,7 @@
       <c r="C14" s="69"/>
       <c r="D14" s="92"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
@@ -3429,7 +3432,7 @@
       <c r="C15" s="69"/>
       <c r="D15" s="92"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
@@ -3437,7 +3440,7 @@
       <c r="C16" s="69"/>
       <c r="D16" s="92"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
@@ -3445,7 +3448,7 @@
       <c r="C17" s="69"/>
       <c r="D17" s="92"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
@@ -3453,7 +3456,7 @@
       <c r="C18" s="94"/>
       <c r="D18" s="95"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <v>0.5</v>
       </c>
@@ -3463,25 +3466,25 @@
       <c r="C19" s="48"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="52"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
@@ -3491,7 +3494,7 @@
       <c r="C23" s="89"/>
       <c r="D23" s="90"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
@@ -3499,7 +3502,7 @@
       <c r="C24" s="69"/>
       <c r="D24" s="92"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
@@ -3507,7 +3510,7 @@
       <c r="C25" s="69"/>
       <c r="D25" s="92"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
@@ -3515,7 +3518,7 @@
       <c r="C26" s="69"/>
       <c r="D26" s="92"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
@@ -3523,7 +3526,7 @@
       <c r="C27" s="69"/>
       <c r="D27" s="92"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
@@ -3531,7 +3534,7 @@
       <c r="C28" s="94"/>
       <c r="D28" s="95"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>0.60416666666666696</v>
       </c>
@@ -3541,7 +3544,7 @@
       <c r="C29" s="69"/>
       <c r="D29" s="70"/>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>0.61458333333333304</v>
       </c>

</xml_diff>

<commit_message>
13:57 - 11.02.2025 - Week 2 coding checking
</commit_message>
<xml_diff>
--- a/NachDurchlaufplan/excelFiles/2-P&DS.xlsx
+++ b/NachDurchlaufplan/excelFiles/2-P&DS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/pit5lo_bosch_com/Documents/Ausbildung - Fachinformatik/NachDurchlaufplan/excelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fachinformatiker-Ausbildung\NachDurchlaufplan\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="307" documentId="13_ncr:1_{34DBF14C-E358-4AB5-A6F9-5FA28043C4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB570772-F56C-4885-83E0-E399D91098DA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676B4C53-2C55-4DD7-8BBB-775D66234210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
+    <workbookView minimized="1" xWindow="1845" yWindow="1830" windowWidth="17250" windowHeight="8865" firstSheet="1" activeTab="3" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -1226,188 +1226,188 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1766,22 +1766,22 @@
       <selection activeCell="B29" sqref="B29:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
@@ -1803,7 +1803,7 @@
       <c r="C3" s="14"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
@@ -1811,25 +1811,25 @@
       <c r="C4" s="15"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-    </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="47"/>
-    </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>0.375</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="C7" s="15"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>0.38541666666666702</v>
       </c>
@@ -1845,7 +1845,7 @@
       <c r="C8" s="15"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>0.39583333333333298</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="C9" s="15"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>0.40625</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="C10" s="15"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>0.41666666666666702</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="C11" s="15"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>0.42708333333333298</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="C12" s="15"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>0.4375</v>
       </c>
@@ -1885,7 +1885,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>0.44791666666666702</v>
       </c>
@@ -1893,7 +1893,7 @@
       <c r="C14" s="15"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>0.45833333333333298</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="C15" s="15"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>0.46875</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="C16" s="15"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>0.47916666666666702</v>
       </c>
@@ -1917,7 +1917,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>0.48958333333333298</v>
       </c>
@@ -1925,35 +1925,35 @@
       <c r="C18" s="15"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="51">
         <v>0.5</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="53"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>0.54166666666666696</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="C23" s="15"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>0.55208333333333304</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>0.5625</v>
       </c>
@@ -1977,7 +1977,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>0.57291666666666696</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>0.58333333333333304</v>
       </c>
@@ -1993,7 +1993,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>0.59375</v>
       </c>
@@ -2001,23 +2001,23 @@
       <c r="C28" s="17"/>
       <c r="D28" s="21"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
-    </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2039,24 +2039,24 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:4" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2070,89 +2070,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="67"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-    </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
-    </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="71"/>
+    </row>
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>0.375</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="62" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="20"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="62"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="58"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="30" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
-      <c r="B10" s="71"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="54" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="29" t="s">
@@ -2160,178 +2160,179 @@
       </c>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B12" s="58"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="30" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="58"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="54"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="31" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="60" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="60"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="21"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="62" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="24"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="63"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="25"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="51">
         <v>0.5</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="53"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="62" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="62"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="62"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="62"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="62" t="s">
+      <c r="B27" s="66"/>
+      <c r="C27" s="63" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="62"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="63"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="64"/>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B30:D30"/>
@@ -2348,7 +2349,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B5:D6"/>
     <mergeCell ref="B19:D22"/>
-    <mergeCell ref="B7:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2358,28 +2358,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C1958D-7396-4A88-8B63-5928A8A1F579}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C15"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:4" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2393,181 +2393,181 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="62" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="62"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="62"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="62"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="63"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>0.375</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="62"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="62"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="62"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="63"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="63"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="62" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="74"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="21"/>
     </row>
-    <row r="13" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="62" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="20"/>
     </row>
-    <row r="14" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="62"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="63"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="62"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="62" t="s">
+      <c r="B16" s="66"/>
+      <c r="C16" s="63" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="62"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="63"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="51">
         <v>0.5</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="53"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="65" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="29" t="s">
@@ -2575,81 +2575,74 @@
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="65"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="62" t="s">
+      <c r="B25" s="66"/>
+      <c r="C25" s="63" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="74"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="73"/>
       <c r="D26" s="21"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="64" t="s">
+      <c r="B27" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="20"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="62"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="63"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="64"/>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="35">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="72"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:D22"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="B3:B10"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="B13:B18"/>
@@ -2658,6 +2651,13 @@
     <mergeCell ref="C27:C29"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:D22"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="B3:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2667,28 +2667,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838E9BEF-82DD-4851-A0DE-5B88C1E3608B}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:4" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2702,11 +2702,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="54" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -2714,251 +2714,246 @@
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="27" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="58"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="58"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>0.375</v>
       </c>
-      <c r="B7" s="58"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="28" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="21"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="36"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="37"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="80"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="38"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="82" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="20"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="82"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="83"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="82"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="83"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="82"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="82"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="83"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="84"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="51">
         <v>0.5</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="53"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="62" t="s">
         <v>57</v>
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="62"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="62"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="62"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="63"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="16"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="64" t="s">
+      <c r="B28" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="62" t="s">
         <v>59</v>
       </c>
       <c r="D28" s="20"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="99"/>
-    </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="35">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="72"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="B19:D22"/>
@@ -2967,6 +2962,11 @@
     <mergeCell ref="C8:C12"/>
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C18"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2980,24 +2980,24 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:4" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3011,91 +3011,91 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>0.375</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="21"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="87" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="20"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>0.40625</v>
       </c>
-      <c r="B10" s="58"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="85"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="54"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="86"/>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="55" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="85" t="s">
@@ -3103,165 +3103,160 @@
       </c>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="58"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="85"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="54"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="86"/>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="60" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="60"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="60"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="67"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="51">
         <v>0.5</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="53"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="62" t="s">
         <v>61</v>
       </c>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="62"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="62"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="62"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="62" t="s">
+      <c r="B27" s="66"/>
+      <c r="C27" s="63" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="62"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="99"/>
-    </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="35">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C27:C29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A19:A22"/>
@@ -3272,6 +3267,11 @@
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C27:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3285,24 +3285,24 @@
       <selection activeCell="B23" sqref="B23:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:4" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3316,241 +3316,241 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>0.34375</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
       <c r="D5" s="30"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="73" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="30"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>0.375</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="30"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="87"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>0.40625</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98"/>
-    </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="98"/>
+      <c r="D10" s="99"/>
+    </row>
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="89"/>
-      <c r="D11" s="90"/>
-    </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
+    </row>
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="92"/>
-    </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="92"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="93"/>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="92"/>
-    </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="92"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="93"/>
+    </row>
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B14" s="91"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="92"/>
-    </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="92"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="93"/>
+    </row>
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B15" s="91"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="92"/>
-    </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="92"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="93"/>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B16" s="91"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="92"/>
-    </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="92"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="93"/>
+    </row>
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B17" s="91"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="92"/>
-    </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="92"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="93"/>
+    </row>
+    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="94"/>
-      <c r="D18" s="95"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50">
+      <c r="B18" s="94"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="96"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="51">
         <v>0.5</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="53"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="90"/>
-    </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="90"/>
+      <c r="D23" s="91"/>
+    </row>
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="92"/>
-    </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="92"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="93"/>
+    </row>
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>0.5625</v>
       </c>
-      <c r="B25" s="91"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="92"/>
-    </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="92"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="93"/>
+    </row>
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="92"/>
-    </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="92"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="93"/>
+    </row>
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="92"/>
-    </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="92"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="93"/>
+    </row>
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>0.59375</v>
       </c>
-      <c r="B28" s="93"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="95"/>
-    </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="94"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="96"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="69"/>
-      <c r="D29" s="70"/>
-    </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="70"/>
+      <c r="D29" s="71"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>